<commit_message>
Realice la primera relacion del contexto Residentes con Reservas la cual tiene el numero reserva-0001 mas unos cambios en las hojas de excel
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquecido Residentes.xlsx
+++ b/Doo-Doc/Seccion # 6/Modelo De Dominio Enriquecido Residentes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/DOO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40778CB9-136A-490C-8094-76459A09212A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629B3AF0-EE2C-4240-8F0D-2C3AE9038C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{007C2ECE-7E90-4717-B1E7-3A143C146FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="1" r:id="rId1"/>
@@ -1328,7 +1328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="95">
   <si>
     <t>Tipo Objeto Dominio</t>
   </si>
@@ -1477,9 +1477,6 @@
     <t>Representa el nombre de un residente determinado.</t>
   </si>
   <si>
-    <t>telefonoCelular</t>
-  </si>
-  <si>
     <t>sólo números enteros</t>
   </si>
   <si>
@@ -1492,12 +1489,6 @@
     <t>Inmueble</t>
   </si>
   <si>
-    <t>Tipo inmueble</t>
-  </si>
-  <si>
-    <t>Representa un objeto tipo inmueble</t>
-  </si>
-  <si>
     <t>Combinaciones únicas</t>
   </si>
   <si>
@@ -1573,45 +1564,18 @@
     <t>Tipo ZonaHabitada</t>
   </si>
   <si>
-    <t>estadoPago</t>
-  </si>
-  <si>
-    <t>lógico</t>
-  </si>
-  <si>
-    <t>sólo un valor lógico</t>
-  </si>
-  <si>
-    <t>Representa el estado de pago de la administración para un inmueble determinado.</t>
-  </si>
-  <si>
     <t>Representa un objeto de tipo ZonaHabitada.</t>
   </si>
   <si>
-    <t>numeroResidentes</t>
-  </si>
-  <si>
     <t>sólo un numero entero</t>
   </si>
   <si>
     <t>Representa el número de residentes que habitan dentro de un mismo inmueble.</t>
   </si>
   <si>
-    <t>estadoInmueble</t>
-  </si>
-  <si>
-    <t>Representa el estado de ocupación de un inmueble.</t>
-  </si>
-  <si>
-    <t>identificador de inmueble</t>
-  </si>
-  <si>
     <t>Identificador</t>
   </si>
   <si>
-    <t>idInmueble</t>
-  </si>
-  <si>
     <t>Representa el nombre o forma común con la que se conoce un inmueble determinado.</t>
   </si>
   <si>
@@ -1621,22 +1585,34 @@
     <t>id de inmueble en zona habitada</t>
   </si>
   <si>
-    <t>numeroInmuebles</t>
-  </si>
-  <si>
     <t>Representa el nombre o forma común con la que se conoce una zona habitada determinada.</t>
   </si>
   <si>
-    <t>Representa el número de inmuebles que hay dentro de una misma zona habitada.</t>
-  </si>
-  <si>
     <t>identificador de zona habitada</t>
   </si>
   <si>
     <t>No es posible tener más de una zona habitada con el mismo numero de identificación.</t>
   </si>
   <si>
-    <t>No es posible tener más de un inmueble con el mismo numero de identificación.</t>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>ConjuntoResidencial</t>
+  </si>
+  <si>
+    <t>conjuntoResidencial</t>
+  </si>
+  <si>
+    <t>xxxxxxxxxxxxxxxxxx@xxxxxxxxx.com  donde cada x representa un digito del 0 al 9 o una letra de la "A" a la "Z" y debe terminas en .com o .co</t>
+  </si>
+  <si>
+    <t>Representa el correo del residente el cual va a realizar la reserva.</t>
+  </si>
+  <si>
+    <t>numeroVivienda</t>
   </si>
 </sst>
 </file>
@@ -2048,14 +2024,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2069,93 +2039,195 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2165,45 +2237,21 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2213,39 +2261,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2256,25 +2271,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2286,22 +2283,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2313,21 +2307,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2727,82 +2706,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="61"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2818,7 +2797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A6ACC7-AE51-45F9-85DD-14DA0E6BE0E5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -2839,78 +2818,78 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="21.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="62"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="str">
+      <c r="D3" s="14" t="str">
         <f>$B$1</f>
         <v>Residentes</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="18" t="str">
+      <c r="D4" s="14" t="str">
         <f>$B$1</f>
         <v>Residentes</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="A5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="str">
+      <c r="D5" s="14" t="str">
         <f>$B$1</f>
         <v>Residentes</v>
       </c>
@@ -2929,1288 +2908,1245 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CD2E3E-2179-4007-8743-BED3F3BF1317}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="69" t="str">
         <f>'Listado Objetos de Dominio'!A3</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="70" t="str">
         <f>'Listado Objetos de Dominio'!B3</f>
         <v>Objeto de dominio que representa a un residente que podrá realizar una reserva de una zona común dentro de un conjunto residencial.</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="26" t="str">
-        <f>A16</f>
+      <c r="R4" s="19" t="str">
+        <f>A18</f>
         <v>Reponsabilidad 1</v>
       </c>
-      <c r="S4" s="27" t="str">
-        <f>A17</f>
+      <c r="S4" s="20" t="str">
+        <f>A19</f>
         <v>Reponsabilidad 2</v>
       </c>
-      <c r="T4" s="28" t="str">
-        <f>A18</f>
+      <c r="T4" s="21" t="str">
+        <f>A20</f>
         <v>Reponsabilidad 3</v>
       </c>
-      <c r="U4" s="29" t="str">
-        <f>A19</f>
+      <c r="U4" s="22" t="str">
+        <f>A21</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="24">
         <v>32</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="24">
         <v>32</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34" t="s">
+      <c r="J5" s="24"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="38"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="31"/>
     </row>
     <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="24">
         <v>1</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="24">
         <v>50</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="33" t="s">
+      <c r="J6" s="24"/>
+      <c r="K6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="38"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="31"/>
     </row>
     <row r="7" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32" t="s">
+      <c r="J7" s="24"/>
+      <c r="K7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="33" t="s">
+      <c r="L7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="34" t="s">
+      <c r="R7" s="28"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="31"/>
+    </row>
+    <row r="8" spans="1:21" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
+        <v>50</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="M8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="31" t="s">
+      <c r="O8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="32" t="s">
+      <c r="P8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="B9" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="31"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31" t="s">
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" s="32" t="s">
+      <c r="B13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="38"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+    </row>
+    <row r="14" spans="1:21" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="B14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="C14" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="45" t="s">
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="L16" s="75"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49" t="s">
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="S16" s="78"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="76"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49" t="s">
+      <c r="K17" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="S14" s="50"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53" t="s">
+      <c r="Q17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="S17" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="53" t="s">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="Q15" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="53" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="40"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="S15" s="54" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="46"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="82" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="52"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="58"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="67"/>
-      <c r="S17" s="68"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="77"/>
-      <c r="S18" s="78"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="86"/>
-      <c r="R19" s="86"/>
-      <c r="S19" s="87"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="89"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="89"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="L17:O17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="L18:O18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="L19:O19"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="L15:O15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="L17:O17"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="C16:G17"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="P16:Q16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{475DC609-B6D5-4D2D-A170-5000DA801120}"/>
-    <hyperlink ref="I19" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{76F12625-B198-4C45-B316-89AD33070AE0}"/>
+    <hyperlink ref="I21" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{76F12625-B198-4C45-B316-89AD33070AE0}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{4616484A-1A8A-4DB6-940E-8291C6AB0942}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{E3F528BF-39F4-4A77-A086-121A7620B9F7}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{84031BE7-BD4B-4472-A1D3-49634C93D82C}"/>
-    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{57BB2E48-0EF6-4E31-8A3C-C7CC98745FF9}"/>
-    <hyperlink ref="A16:B16" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{A7849B7E-A984-439D-AC57-2AF622631983}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{BA0AA56C-D662-4271-912B-1B000C27B93A}"/>
+    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{57BB2E48-0EF6-4E31-8A3C-C7CC98745FF9}"/>
+    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{A7849B7E-A984-439D-AC57-2AF622631983}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{BA0AA56C-D662-4271-912B-1B000C27B93A}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{B80B22E6-6928-44D7-BF33-2D2339A3EAD3}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{2CEFD9A1-7256-4CC0-A14B-05D2869A5C81}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{35AD5D22-1DAF-4594-AD05-7CB9953F9873}"/>
-    <hyperlink ref="C12" location="Residente!B2" display="Residente" xr:uid="{44C56CF5-7141-4A21-B9BC-308CD3AA36CE}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{35AD5D22-1DAF-4594-AD05-7CB9953F9873}"/>
+    <hyperlink ref="C14" location="Residente!A5" display="identificador" xr:uid="{44C56CF5-7141-4A21-B9BC-308CD3AA36CE}"/>
+    <hyperlink ref="I8" r:id="rId1" xr:uid="{DB94A35C-D1D9-4791-A75D-DEEACCA61A6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2C0303-B4E7-4897-A4E9-4C4FB55D2E79}">
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="69" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Inmueble</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="70" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada uno de los inmbuebles dónde viven los residentes dentro de un conjunto residencial para generar reservas.</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="26" t="str">
-        <f>A21</f>
+      <c r="R4" s="19" t="str">
+        <f>A17</f>
         <v>Reponsabilidad 1</v>
       </c>
-      <c r="S4" s="27" t="str">
-        <f>A22</f>
+      <c r="S4" s="20" t="str">
+        <f>A18</f>
         <v>Reponsabilidad 2</v>
       </c>
-      <c r="T4" s="28" t="str">
-        <f>A23</f>
+      <c r="T4" s="21" t="str">
+        <f>A19</f>
         <v>Reponsabilidad 3</v>
       </c>
-      <c r="U4" s="29" t="str">
-        <f>A24</f>
+      <c r="U4" s="22" t="str">
+        <f>A20</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="24">
         <v>32</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="24">
         <v>32</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34" t="s">
+      <c r="J5" s="24"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="38"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="31"/>
     </row>
     <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="24">
         <v>1</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="24">
         <v>50</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="33" t="s">
+      <c r="J6" s="24"/>
+      <c r="K6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="R6" s="28"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="31"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="38"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="34" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="M7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="31" t="s">
+      <c r="O7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
+      <c r="Q7" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7" s="28"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="31"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32" t="s">
+      <c r="A8" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="28"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q8" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="38"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N9" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O9" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="38"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N10" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="P10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="R10" s="35"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="38"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="41"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="43" t="s">
+      <c r="C12" s="58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="91"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="90" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="89"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="93" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="94" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="95"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="94" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="75"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="75"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="78"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="76"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q16" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="S16" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="80"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="40"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="65"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="46"/>
+    </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49" t="s">
-        <v>62</v>
-      </c>
+      <c r="A19" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="48"/>
       <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="S19" s="50"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="52"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="52"/>
-      <c r="P20" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q20" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="S20" s="54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="55" t="s">
+      <c r="A20" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="58"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="68"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="78"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="85"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="85"/>
-      <c r="O24" s="85"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="86"/>
-      <c r="R24" s="86"/>
-      <c r="S24" s="87"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="R19:S19"/>
+  <mergeCells count="25">
+    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="L20:O20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="L17:O17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:G16"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{9D0395C4-6CFD-4925-83D2-133B3276059C}"/>
-    <hyperlink ref="I24" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{0BB46161-5CF1-4CF8-B1D9-64C89E7CF0EA}"/>
+    <hyperlink ref="I20" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{0BB46161-5CF1-4CF8-B1D9-64C89E7CF0EA}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{281E9218-6D02-472C-85C4-F6B085CD882E}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{BC879403-9FDA-4042-B8F7-DD5D346297D1}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{06202D81-809E-4E1E-8A24-FF90F053F4D3}"/>
-    <hyperlink ref="A22:B22" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{12200A77-9952-4B84-8945-AB97647F9C95}"/>
-    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{1FBD4C26-5BA4-4489-A75C-BA3637B08199}"/>
-    <hyperlink ref="A24:B24" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{F36C0CE1-7DFD-49C3-853F-960D9A7FEEE4}"/>
+    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{12200A77-9952-4B84-8945-AB97647F9C95}"/>
+    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{1FBD4C26-5BA4-4489-A75C-BA3637B08199}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{F36C0CE1-7DFD-49C3-853F-960D9A7FEEE4}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{5FA9620C-6914-4832-8F9B-FF75CEBE5941}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{B3CAC922-3E95-4652-A4AF-75A08339FC25}"/>
-    <hyperlink ref="A23:B23" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{88D92FFC-262A-4889-866C-1093A1FC4078}"/>
-    <hyperlink ref="C15" location="Inmueble!A6" display="idInmueble" xr:uid="{2046AD99-A820-4B2D-AFAF-0EA494A6B78C}"/>
-    <hyperlink ref="C14" location="Inmueble!A5" display="Identificador" xr:uid="{408169EF-EAE2-4A46-92B2-54B1094CF953}"/>
-    <hyperlink ref="C16" location="Inmueble!A6" display="idInmueble" xr:uid="{AAF50891-00A3-490F-868D-CBD9FF3BFA47}"/>
-    <hyperlink ref="C17" location="Inmueble!A10" display="ZonaHabitada" xr:uid="{6D0CBE6B-5404-456E-A8E0-AA3E78885F1D}"/>
+    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{88D92FFC-262A-4889-866C-1093A1FC4078}"/>
+    <hyperlink ref="C12" location="Inmueble!A5" display="identificador" xr:uid="{AAF50891-00A3-490F-868D-CBD9FF3BFA47}"/>
+    <hyperlink ref="C13" location="Inmueble!A8" display="ZonaHabitada" xr:uid="{6D0CBE6B-5404-456E-A8E0-AA3E78885F1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4219,554 +4155,513 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE91583B-F698-4020-97FF-1414BFE2C5EB}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.33203125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="79.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="94.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="132.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="66.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="52.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.44140625" style="12"/>
+    <col min="1" max="1" width="23.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="79.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="94.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="132.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="66.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.44140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21" t="str">
+      <c r="B2" s="69" t="str">
         <f>'Listado Objetos de Dominio'!A5</f>
         <v>ZonaHabitada</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="70" t="str">
         <f>'Listado Objetos de Dominio'!B5</f>
         <v>Objeto de dominio que representa a cada una de las zonas habitadas que se encuentran dentro de un conjunto residencial para que los residentes puedan identificar la zona dónde se encuentra el inmueble.</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="26" t="str">
+      <c r="R4" s="19" t="str">
+        <f>A15</f>
+        <v>Reponsabilidad 1</v>
+      </c>
+      <c r="S4" s="20" t="str">
         <f>A16</f>
-        <v>Reponsabilidad 1</v>
-      </c>
-      <c r="S4" s="27" t="str">
+        <v>Reponsabilidad 2</v>
+      </c>
+      <c r="T4" s="21" t="str">
         <f>A17</f>
-        <v>Reponsabilidad 2</v>
-      </c>
-      <c r="T4" s="28" t="str">
+        <v>Reponsabilidad 3</v>
+      </c>
+      <c r="U4" s="22" t="str">
         <f>A18</f>
-        <v>Reponsabilidad 3</v>
-      </c>
-      <c r="U4" s="29" t="str">
-        <f>A19</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="24">
         <v>32</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="24">
         <v>32</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34" t="s">
+      <c r="J5" s="24"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="38"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="31"/>
     </row>
     <row r="6" spans="1:21" ht="69" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="24">
         <v>1</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="24">
         <v>50</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="33" t="s">
+      <c r="J6" s="24"/>
+      <c r="K6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="38"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32" t="s">
+      <c r="Q6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="R6" s="28"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="31"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q7" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="R7" s="35"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="38"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="43" t="s">
+      <c r="C10" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="95"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="90" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="89"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="75"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="S13" s="78"/>
+    </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="76"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49" t="s">
+      <c r="K14" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="S14" s="50"/>
+      <c r="Q14" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="S14" s="39" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="53" t="s">
+      <c r="A15" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="Q15" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="53" t="s">
+      <c r="B15" s="80"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="40"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="S15" s="54" t="s">
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="46"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="82" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="55" t="s">
+      <c r="B17" s="83"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="85"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="52"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="58"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="67"/>
-      <c r="S17" s="68"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="77"/>
-      <c r="S18" s="78"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="86"/>
-      <c r="R19" s="86"/>
-      <c r="S19" s="87"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="L19:O19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="L18:O18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="L16:O16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="L17:O17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="L18:O18"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
     <mergeCell ref="L15:O15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:G15"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="C13:G14"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:O13"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{2CE3EBFB-A4E8-4C22-9348-9D6C0442B5B7}"/>
-    <hyperlink ref="I19" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{E4777A3B-7BC1-41D1-B1FE-D03702A7CF3A}"/>
+    <hyperlink ref="I18" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{E4777A3B-7BC1-41D1-B1FE-D03702A7CF3A}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{B0C7580D-0EE9-4D0A-9351-79C142125532}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{1FAC0AD2-A92C-49E6-BDE9-1F7E75529655}"/>
     <hyperlink ref="U4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{C7658912-3AD4-456C-B65D-150528D00C6B}"/>
-    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{6B3D46C6-B186-42C5-BC8D-8BC01FF53662}"/>
-    <hyperlink ref="A16:B16" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{5EBF8D4C-C36E-4E97-916A-844456BD3018}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{B3A4E974-ECAF-43F1-84EB-8C54605A351E}"/>
+    <hyperlink ref="A16:B16" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{6B3D46C6-B186-42C5-BC8D-8BC01FF53662}"/>
+    <hyperlink ref="A15:B15" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{5EBF8D4C-C36E-4E97-916A-844456BD3018}"/>
+    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{B3A4E974-ECAF-43F1-84EB-8C54605A351E}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{BB51BE81-EE9C-42ED-B56B-C34D94C2EE12}"/>
     <hyperlink ref="A1:Q1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{761F0984-1BC0-491D-960F-97958134D35B}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{DF67632F-243F-40C9-9C66-F3761BB6CC27}"/>
-    <hyperlink ref="C12" location="Inmueble!A6" display="idInmueble" xr:uid="{5718E767-3AE8-4633-BD09-9CF59FB23377}"/>
-    <hyperlink ref="C11" location="Inmueble!A5" display="Identificador" xr:uid="{E689A8A3-2FE6-4452-8F8E-9C7F29EEF6E0}"/>
+    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{DF67632F-243F-40C9-9C66-F3761BB6CC27}"/>
+    <hyperlink ref="C11" location="ZonaHabitada!A6" display="nombre" xr:uid="{5718E767-3AE8-4633-BD09-9CF59FB23377}"/>
+    <hyperlink ref="C10" location="ZonaHabitada!A5" display="Identificador" xr:uid="{E689A8A3-2FE6-4452-8F8E-9C7F29EEF6E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>